<commit_message>
alteracoes no dicionario '
</commit_message>
<xml_diff>
--- a/DicionarioDeDados-DependenciasCorrespondentesCanais.xlsx
+++ b/DicionarioDeDados-DependenciasCorrespondentesCanais.xlsx
@@ -1,25 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSDS\Documents\GitHub\Open-Banking-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loro\source\openbanking-febraban\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6F8D77-5960-492D-AB92-653776B32A2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dependências-Agências" sheetId="1" r:id="rId1"/>
     <sheet name="Correspondentes" sheetId="2" r:id="rId2"/>
     <sheet name="CanaisAtendimentoEletrônicos" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -648,7 +657,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1188,14 +1197,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1855,7 +1864,7 @@
     </row>
     <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="39" t="str">
-        <f t="shared" ref="A19:A26" si="1">CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/Companies/Branches/Availability/Standard/",B19)</f>
+        <f t="shared" ref="A19:A25" si="1">CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/Companies/Branches/Availability/Standard/",B19)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/Companies/Branches/Availability/Standard/WeekdayName</v>
       </c>
       <c r="B19" s="39" t="s">
@@ -2232,7 +2241,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
@@ -3356,7 +3365,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">

</xml_diff>

<commit_message>
Atualizações após reuniões com os DOs em 08/07
Atualizações gerais nos dicionários de dados.
</commit_message>
<xml_diff>
--- a/DicionarioDeDados-DependenciasCorrespondentesCanais.xlsx
+++ b/DicionarioDeDados-DependenciasCorrespondentesCanais.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020"/>
   </bookViews>
   <sheets>
     <sheet name="Dependências-Agências" sheetId="1" r:id="rId1"/>
@@ -1054,11 +1054,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1788,65 +1788,67 @@
     </row>
     <row r="21" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/availability/standard/type</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/branches/availability/standard/",B21)</f>
+        <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/availability/standard/allowPublicAccess</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="13">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="I21" s="9">
+        <v>1</v>
+      </c>
+      <c r="J21" s="9">
+        <v>1</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L21" s="11"/>
+    </row>
+    <row r="22" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/branches/availability/phones/",B22)</f>
+        <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/availability/phones/type</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C22" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E21" s="13">
-        <v>1</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="I21" s="9">
-        <v>0</v>
-      </c>
-      <c r="J21" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="L21" s="11"/>
-    </row>
-    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/availability/standard/areaCode</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="E22" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H22" s="3"/>
+      <c r="G22" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="I22" s="9">
         <v>0</v>
       </c>
@@ -1854,32 +1856,32 @@
         <v>18</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L22" s="11"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/availability/standard/number</v>
+        <f t="shared" ref="A23:A24" si="3">CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/branches/availability/phones/",B23)</f>
+        <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/availability/phones/areaCode</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E23" s="13">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="16" t="s">
-        <v>17</v>
+      <c r="G23" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="9">
@@ -1889,41 +1891,39 @@
         <v>18</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="L23" s="11"/>
     </row>
-    <row r="24" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/availability/standard/allowPublicAccess</v>
+        <f t="shared" si="3"/>
+        <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/availability/phones/number</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>76</v>
+        <v>33</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>79</v>
+        <v>14</v>
       </c>
       <c r="E24" s="13">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>78</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="3"/>
       <c r="I24" s="9">
-        <v>1</v>
-      </c>
-      <c r="J24" s="9">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="K24" s="8" t="s">
         <v>19</v>
@@ -3076,11 +3076,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Ajustes a pedido do GT Dados
Retirado o tradingName (nome fantasia) da empresa do correspondente e deixado o conglomerado, a qual pertence o correspondente, como opcional.
</commit_message>
<xml_diff>
--- a/DicionarioDeDados-DependenciasCorrespondentesCanais.xlsx
+++ b/DicionarioDeDados-DependenciasCorrespondentesCanais.xlsx
@@ -1,32 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23107"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSDS\Documents\GitHub\Open-Banking-\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED0C5B61-5A09-4718-BC60-394F6CA166C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dependências-Agências" sheetId="1" r:id="rId1"/>
     <sheet name="Correspondentes" sheetId="2" r:id="rId2"/>
     <sheet name="CanaisAtendimentoEletrônicos" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="118">
   <si>
     <t>Xpath</t>
   </si>
@@ -61,124 +70,41 @@
     <t>Restrições</t>
   </si>
   <si>
-    <t>Opcional</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nome do conglomerado proprietário da dependência (titular). Ex. 'Organização A' </t>
+  </si>
+  <si>
+    <t>Texto</t>
   </si>
   <si>
     <t>Mandatório</t>
   </si>
   <si>
-    <t>Campo de texto livre para descrever mais sobre os serviços</t>
-  </si>
-  <si>
-    <t>Texto</t>
-  </si>
-  <si>
     <t>\w*\W*</t>
   </si>
   <si>
-    <t>(\d{5})-(\d{3})</t>
-  </si>
-  <si>
-    <t>([0-9]{4,5})-([0-9]{4})</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>Número de DDD (Discagem Direta à Distância) do telefone da 
-dependência - se houver. Ex. '19'</t>
-  </si>
-  <si>
-    <t>Número de DDD (Discagem Direta à Distância) para  telefone de acesso ao Canal - se houver. Ex. '19'</t>
-  </si>
-  <si>
-    <t>Logradouro é o termo utilizado pelos Correios para designar uma localidade específica. O logradouro é composto pelo seu tipo seguido dos nomes oficiais. Os tipos de logradouro são: aeroporto, alameda, área, avenida, campo, chácara, colônia, condomínio, conjunto, distrito, esplanada, estação, estrada, fazenda, feira, jardim, ladeira, lago, lagoa ,largo, loteament, núcleo, parque, passarela, pátio, praça, quadra, recanto, residencial, rodovia, rua, setor, sítio, travessa, trecho, trevo, vale, vereda, via, viaduto, viela, vila</t>
-  </si>
-  <si>
-    <t>Os logradouros são identificados pelo nome oficial atribuído pelo município ao qual estão vinculados. Exemplo: Avenida Paulista, sendo “Avenida” o tipo e “Paulista” o nome do logradouro</t>
-  </si>
-  <si>
-    <t>Bairro é uma comunidade ou região localizada em uma cidade ou município de acordo com as suas subdivisões geográficas. Exemplo: 'Paraíso'</t>
-  </si>
-  <si>
-    <t>Código de Endereçamento Postal: Composto por um conjunto numérico de oito dígitos, o objetivo principal do CEP é orientar e acelerar o encaminhamento, o tratamento e a entrega de objetos postados nos Correios, por meio da sua atribuição a localidades, logradouros, unidades dos Correios, serviços, órgãos públicos, empresas e edifícios. Ex. '01311-000'</t>
-  </si>
-  <si>
-    <t>Números de 0 a 9</t>
-  </si>
-  <si>
-    <t>(Domingo)|(Segunda-feira)|(Terça-feira)|(Quarta-feira)|(Quinta-feira)|(Sexta-feira)|(Sábado)</t>
-  </si>
-  <si>
-    <t>Em formato texto, seguindo o domínio apresentado, devem ser colocados os dias da semana.</t>
-  </si>
-  <si>
-    <t>Segunda-Feira
-Terça-Feira
-Quarta-Feira
-Quinta-Feira
-Sexta-Feira</t>
-  </si>
-  <si>
-    <t>O número especifica o imóvel. Ocorrem, raras vezes, de o imóvel não ter número. Para os logradouros sem numeração recomenda-se a utilização da sigla 's/n'.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Localidade: O nome da localidade corresponde à designação da cidade ou município no qual o endereço está localizado. Ex. 'São Paulo'
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Localidade: O nome da localidade corresponde à designação
-da cidade ou município no qual o endereço está localizado. Ex. 'São Paulo'
-</t>
-  </si>
-  <si>
-    <t>Número de telefone da dependência - se houver</t>
-  </si>
-  <si>
-    <t>^\d{4}$</t>
-  </si>
-  <si>
-    <t>^\d{2}$</t>
-  </si>
-  <si>
-    <t>^(\d{5})-(\d{3})$</t>
-  </si>
-  <si>
-    <t>Dígito verificador do código da dependência</t>
-  </si>
-  <si>
-    <t>Alguns logradouros ainda necessitam ser especificados por meio de complemento, conforme o exemplo a seguir: 'Loja B', 'Fundos', 'Casa 2', 'Lote C'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Texto
-</t>
-  </si>
-  <si>
-    <t>Logradouro é o termo utilizado pelos Correios para designar uma localidade específica. O logradouro é composto pelo seu tipo seguido dos nomes oficiais. Os tipos de logradouro são: aeroporto, alameda, área, avenida, campo, chácara, colônia, condomínio, conjunto, distrito, esplanada, estação, estrada, fazenda, feira, jardim, ladeira, lago, lagoa ,largo, loteamento, núcleo, parque, passarela, pátio, praça, quadra, recanto, residencial, rodovia, rua, setor, sítio, travessa, trecho, trevo, vale, vereda, via, viaduto, viela, vila</t>
-  </si>
-  <si>
-    <t>Os tipos de logradouro são: aeroporto, alameda, área, avenida, campo, chácara, colônia, condomínio, conjunto, distrito, esplanada, estação, estrada, fazenda, feira, jardim, ladeira, lago, lagoa ,largo, loteamento, núcleo, parque, passarela, pátio, praça, quadra, recanto, residencial, rodovia, rua, setor, sítio, travessa, trecho, trevo, vale, vereda, via, viaduto, viela, vila</t>
-  </si>
-  <si>
-    <t>Nome do conglomerado ao qual pertence o agente bancário, por exemplo: 
-"Companhia Brasileira de Distribuição"
-"Empresa Brasileira de Correios e Telegrafos - ECT"
-'Grupo Pão de Açúcar'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serviços prestados pela dependência consultada:
-1. Abertura de contas
-2.Recebimentos, pagamentos e transferências eletrônicas
-3.Recebimentos e pagamentos de qualquer natureza
-4.Operações de crédito
-5.Cartão de crédito
-6.Operações de câmbio
-7.Investimentos
-8.Seguros
-</t>
+    <t>Nome da Instituição, pertencente à organização, responsável pela Dependência. Ex. 'Empresa da Organização A'</t>
+  </si>
+  <si>
+    <t>cnpjNumber</t>
+  </si>
+  <si>
+    <t>Número completo do CNPJ da instituição responsável pela dependência - o CNPJ corresponde ao número de inscrição no Cadastro de Pessoa Jurídica. Os oito primeiros números à esquerda (XX. XXX. XXX) formam a "raiz" ou base, que identifica a empresa de forma única. Ex. '50.685.362'. Os 4 próximos números indicam filial. Os últimos dois dígitos são para o número verificador do CNPJ, calculado em duas etapas utilizando o módulo de divisão 11, utilizando-se os 12 primeiros números do CNPJ - inscrição e filial.
+Deve-se ter apenas os números do CNPJ, sem máscara.</t>
+  </si>
+  <si>
+    <t>^(\d{14})$</t>
+  </si>
+  <si>
+    <t>Números de 0 a 9.</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
   <si>
     <r>
@@ -248,21 +174,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Código identificador da dependência. Ex. '3006','3035', '1382', '2516', '2856'. </t>
-  </si>
-  <si>
-    <t>Para qualquer tipo de dependência informada deverá ser sempre preenchido com a identificação da Agência</t>
-  </si>
-  <si>
-    <t>Em campo texto devem ser registradas todas as Exceções para o não atendimento.  Ex. 'Exceto feriados municipais, nacionais e estaduais'.</t>
-  </si>
-  <si>
-    <t>Horário padrão de início de atendimento da Dependência.
-O horário deve estar no formato UTC (10:00:00+0000).</t>
-  </si>
-  <si>
-    <t>Horário padrão de encerramento de atendimento da Dependência.
-O horário deve estar no formato UTC (16:00:00+0000).</t>
+    <t>Enum</t>
+  </si>
+  <si>
+    <t>^\d{1,2}$</t>
   </si>
   <si>
     <t>1 - Agência
@@ -270,71 +185,31 @@
 3 - Posto de Atendimento Eletrônico</t>
   </si>
   <si>
-    <t>Preenchimento com horário universal (em UTC)</t>
-  </si>
-  <si>
-    <t>^([0|1|2]{1})([0-9]{1}):([0|1|2|3|4|5]{1})([0-9]{1}):([0|1|2|3|4|5]{1})([0-9]{1})\+([0-9]{4})$</t>
-  </si>
-  <si>
-    <t>1 'Recepção e encaminhamento de propostas de abertura de contas'
-2 'Realização de recebimentos, pagamentos e transferências eletrônicas'
-3 'Recebimentos e pagamentos de qualquer natureza'
-4 'Execução ativa e passiva de ordens de pagamento'
-5 'Recepção e encaminhamento de propostas de operações de crédito e de arrendamento mercantil'
-6 'Recebimento e pagamentos relacionados a letras de câmbio de aceite da instituição'
-7 'Recepção e encaminhamento de propostas de fornecimento de cartões de crédito'
-8 'Realização de operações de câmbio'</t>
-  </si>
-  <si>
-    <t>Número de DDI (Discagem Direta Internacional) para  telefone de acesso ao Canal - se houver. Ex. '55'</t>
-  </si>
-  <si>
-    <t>Endereço eletrônico de acesso ao canal. URLs são limitadas a 2048 caracteres mas, para o contexto do Sistema Financeiro aberto, será adotado a metade deste tamanho. Ex. 'https://example.com/mobile-banking'</t>
-  </si>
-  <si>
-    <t>Se houver um número de telefone obrigatoriamente devemos ter seu tipo identificado</t>
-  </si>
-  <si>
-    <t>Se houver um número de telefone obrigatoriamente devemos ter um DDD</t>
-  </si>
-  <si>
-    <t>1. 'Fixo'
-2. 'Móvel"</t>
-  </si>
-  <si>
-    <t>Tipo de canal de atendimento:
-1 'Internet banking'
-2 'Mobile banking' 
-3 'Central telefônica banking'
-4 'SAC'
-5 'Ouvidoria'
-6 'Chat'</t>
-  </si>
-  <si>
-    <t>1 'Internet banking'
-2 'Mobile banking' 
-3 'Central telefônica banking'
-4 'SAC'
-5 'Ouvidoria'
-6 'Chat'</t>
-  </si>
-  <si>
-    <t>^\d{1,2}$</t>
+    <t>code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código identificador da dependência. Ex. '3006','3035', '1382', '2516', '2856'. </t>
+  </si>
+  <si>
+    <t>^\d{4}$</t>
+  </si>
+  <si>
+    <t>Números de 0 a 9</t>
+  </si>
+  <si>
+    <t>Para qualquer tipo de dependência informada deverá ser sempre preenchido com a identificação da Agência</t>
+  </si>
+  <si>
+    <t>checkDigit</t>
+  </si>
+  <si>
+    <t>Dígito verificador do código da dependência</t>
+  </si>
+  <si>
+    <t>Opcional</t>
   </si>
   <si>
     <t>^\d{1}$</t>
-  </si>
-  <si>
-    <t>^([0-9]{1})$</t>
-  </si>
-  <si>
-    <t>Mensagem complementar necessária para o agrupamento da identificação do telefone. Exemplos relativos ao prenchimento do agrupmento telefone: 
-DDI '55'; DDD '11', '40044828, 'Para clientes no exterior'
-DDI ' ', DDD ' ', 40044828', "Para regiões metropolitanas'
-DDI ' ', DDD ' ', 40044828', "Para demais localidades'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nome do conglomerado proprietário da dependência (titular). Ex. 'Organização A' </t>
   </si>
   <si>
     <t xml:space="preserve">Nome da dependência, exemplos: 
@@ -346,43 +221,121 @@
    </t>
   </si>
   <si>
-    <t>Nome do conglomerado responsável pela contrataçao do Correspondente. Ex. 'Organização A</t>
-  </si>
-  <si>
-    <t>Nome do contratante do serviço do correspondente. Ex. 'Empresa Contratante'</t>
-  </si>
-  <si>
-    <t>Nome do Correspondente Bancário. Segundo Glossário do
-Bacen: Correspondentes no pais são Empresas, integrantes ou não do Sistema Financeiro Nacional, contratadas por instituições financeiras e demais instituições autorizadas a funcionar pelo Banco Central do Brasil para a prestação de serviços de atendimento aos clientes e usuários dessas instituições. Os correspondentes mais conhecidos são as lotéricas e o banco postal. Ex. 'Empresa Correspondente S.A.'</t>
-  </si>
-  <si>
-    <t>Nome fantasia do Correspondente. Ex. 'Correspondente Minuto'</t>
-  </si>
-  <si>
-    <t>Nome do conglomerado que disponibiliza os Canais de Atendimento Eletrônico (titular). Ex.  'Organização A'</t>
-  </si>
-  <si>
-    <t>Números de 0 a 9.
-O Tipo de Canal determina o Tipo de Acesso a ele relacionado: 
-1. URL para acesso ao internet banking,
-2. URL para aquisição do app , 
-3. telefone/URL da central, 
-4. telefone/URL do SAC, 
-5. telefone/URL da ouvidoria, 
-6. telefone/URL para chat</t>
-  </si>
-  <si>
-    <t>Identificação do Tipo de telefone da dependência. Ex. 1.Fixo, 2.Móvel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Número de telefone de acesso ao canal. Ex:' 4004-4828', '99878-5342', '0800-778-7788' 
+    <t>streetType</t>
+  </si>
+  <si>
+    <t>Logradouro é o termo utilizado pelos Correios para designar uma localidade específica. O logradouro é composto pelo seu tipo seguido dos nomes oficiais. Os tipos de logradouro são: aeroporto, alameda, área, avenida, campo, chácara, colônia, condomínio, conjunto, distrito, esplanada, estação, estrada, fazenda, feira, jardim, ladeira, lago, lagoa ,largo, loteamento, núcleo, parque, passarela, pátio, praça, quadra, recanto, residencial, rodovia, rua, setor, sítio, travessa, trecho, trevo, vale, vereda, via, viaduto, viela, vila</t>
+  </si>
+  <si>
+    <t>Os tipos de logradouro são: aeroporto, alameda, área, avenida, campo, chácara, colônia, condomínio, conjunto, distrito, esplanada, estação, estrada, fazenda, feira, jardim, ladeira, lago, lagoa ,largo, loteamento, núcleo, parque, passarela, pátio, praça, quadra, recanto, residencial, rodovia, rua, setor, sítio, travessa, trecho, trevo, vale, vereda, via, viaduto, viela, vila</t>
+  </si>
+  <si>
+    <t>streetName</t>
+  </si>
+  <si>
+    <t>Os logradouros são identificados pelo nome oficial atribuído pelo município ao qual estão vinculados. Exemplo: Avenida Paulista, sendo “Avenida” o tipo e “Paulista” o nome do logradouro</t>
+  </si>
+  <si>
+    <t>buildingNumber</t>
+  </si>
+  <si>
+    <t>O número especifica o imóvel. Ocorrem, raras vezes, de o imóvel não ter número. Para os logradouros sem numeração recomenda-se a utilização da sigla 's/n'.</t>
+  </si>
+  <si>
+    <t>additionalInfo</t>
+  </si>
+  <si>
+    <t>Alguns logradouros ainda necessitam ser especificados por meio de complemento, conforme o exemplo a seguir: 'Loja B', 'Fundos', 'Casa 2', 'Lote C'</t>
+  </si>
+  <si>
+    <t>districtName</t>
+  </si>
+  <si>
+    <t>Bairro é uma comunidade ou região localizada em uma cidade ou município de acordo com as suas subdivisões geográficas. Exemplo: 'Paraíso'</t>
+  </si>
+  <si>
+    <t>townName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Localidade: O nome da localidade corresponde à designação
+da cidade ou município no qual o endereço está localizado. Ex. 'São Paulo'
 </t>
   </si>
   <si>
-    <t>^(([0-9]{4,5})-([0-9]{4}))|(([0-9]{4})-([0-9]{3})-([0-9]{4}))$</t>
+    <t>countrySubDivision</t>
+  </si>
+  <si>
+    <t>Enumeração referente a cada sigla da unidade da federação que identifica o estado ou o distrito federal, no qual o endereço está localizado. Ex. 1-'AC'. São considerados apenas as siglas para os estados brasileiros.</t>
+  </si>
+  <si>
+    <t>^(\d{1})$</t>
+  </si>
+  <si>
+    <t>1-'AC'; 2-'AL'; 3-'AM'; 4-'AP'; 5-'BA'; 6-'CE'; 7-'DF'; 8-'ES'; 9-'GO'; 10-'MA'; 11-'MG'; 12-'MS'; 13-'MT'; 14-'PA'; 15-'PB'; 16-'PE'; 17-'PI'; 18-'PR'; 19-'RJ'; 20-'RN'; 21-'RO'; 22-'RR'; 23-'RS'; 24-'SC'; 25-'SE'; 26-'SP'; 27-'TO'</t>
+  </si>
+  <si>
+    <t>postCode</t>
+  </si>
+  <si>
+    <t>Código de Endereçamento Postal: Composto por um conjunto numérico de oito dígitos, o objetivo principal do CEP é orientar e acelerar o encaminhamento, o tratamento e a entrega de objetos postados nos Correios, por meio da sua atribuição a localidades, logradouros, unidades dos Correios, serviços, órgãos públicos, empresas e edifícios. Ex. '01311-000'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Texto
+</t>
+  </si>
+  <si>
+    <t>(\d{5})-(\d{3})</t>
+  </si>
+  <si>
+    <t>weekday</t>
+  </si>
+  <si>
+    <t>Em formato texto, seguindo o domínio apresentado, devem ser colocados os dias da semana.</t>
+  </si>
+  <si>
+    <t>(Domingo)|(Segunda-feira)|(Terça-feira)|(Quarta-feira)|(Quinta-feira)|(Sexta-feira)|(Sábado)</t>
+  </si>
+  <si>
+    <t>Segunda-Feira
+Terça-Feira
+Quarta-Feira
+Quinta-Feira
+Sexta-Feira</t>
+  </si>
+  <si>
+    <t>openingTime</t>
+  </si>
+  <si>
+    <t>Horário padrão de início de atendimento da Dependência.
+O horário deve estar no formato UTC (10:00:00+0000).</t>
+  </si>
+  <si>
+    <t>^([0|1|2]{1})([0-9]{1}):([0|1|2|3|4|5]{1})([0-9]{1}):([0|1|2|3|4|5]{1})([0-9]{1})\+([0-9]{4})$</t>
+  </si>
+  <si>
+    <t>Preenchimento com horário universal (em UTC)</t>
+  </si>
+  <si>
+    <t>closingTime</t>
+  </si>
+  <si>
+    <t>Horário padrão de encerramento de atendimento da Dependência.
+O horário deve estar no formato UTC (16:00:00+0000).</t>
+  </si>
+  <si>
+    <t>exceptionAvailability</t>
+  </si>
+  <si>
+    <t>Em campo texto devem ser registradas todas as Exceções para o não atendimento.  Ex. 'Exceto feriados municipais, nacionais e estaduais'.</t>
+  </si>
+  <si>
+    <t>allowPublicAccess</t>
   </si>
   <si>
     <t>Indica se a dependência tem acesso restrito a clientes, por exemplo, uma agência dentro de uma empresa que só atenda aos clientes daquela empresa, ou acesso irrestrito, atendendo o público em geral.</t>
+  </si>
+  <si>
+    <t>Booleano</t>
   </si>
   <si>
     <t>^\[0-1]{1}$</t>
@@ -392,7 +345,57 @@
 1. Acesso restrito</t>
   </si>
   <si>
-    <t>Booleano</t>
+    <t>Identificação do Tipo de telefone da dependência. Ex. 1.Fixo, 2.Móvel</t>
+  </si>
+  <si>
+    <t>^([0-9]{1})$</t>
+  </si>
+  <si>
+    <t>1. 'Fixo'
+2. 'Móvel"</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Se houver um número de telefone obrigatoriamente devemos ter seu tipo identificado</t>
+  </si>
+  <si>
+    <t>areaCode</t>
+  </si>
+  <si>
+    <t>Número de DDD (Discagem Direta à Distância) do telefone da 
+dependência - se houver. Ex. '19'</t>
+  </si>
+  <si>
+    <t>^\d{2}$</t>
+  </si>
+  <si>
+    <t>Se houver um número de telefone obrigatoriamente devemos ter um DDD</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>Número de telefone da dependência - se houver</t>
+  </si>
+  <si>
+    <t>([0-9]{4,5})-([0-9]{4})</t>
+  </si>
+  <si>
+    <t>codes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serviços prestados pela dependência consultada:
+1. Abertura de contas
+2.Recebimentos, pagamentos e transferências eletrônicas
+3.Recebimentos e pagamentos de qualquer natureza
+4.Operações de crédito
+5.Cartão de crédito
+6.Operações de câmbio
+7.Investimentos
+8.Seguros
+</t>
   </si>
   <si>
     <t>1 'Abertura de contas'
@@ -405,85 +408,47 @@
 8 'Seguros'</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>checkDigit</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>streetType</t>
-  </si>
-  <si>
-    <t>streetName</t>
-  </si>
-  <si>
-    <t>buildingNumber</t>
-  </si>
-  <si>
-    <t>additionalInfo</t>
-  </si>
-  <si>
-    <t>districtName</t>
-  </si>
-  <si>
-    <t>townName</t>
-  </si>
-  <si>
-    <t>postCode</t>
-  </si>
-  <si>
-    <t>weekday</t>
-  </si>
-  <si>
-    <t>openingTime</t>
-  </si>
-  <si>
-    <t>closingTime</t>
-  </si>
-  <si>
-    <t>exceptionAvailability</t>
-  </si>
-  <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>codes</t>
+    <t>Campo de texto livre para descrever mais sobre os serviços</t>
+  </si>
+  <si>
+    <t>Nome do conglomerado responsável pela contrataçao do Correspondente. Ex. 'Organização A</t>
+  </si>
+  <si>
+    <t>Nome do contratante do serviço do correspondente. Ex. 'Empresa Contratante'</t>
+  </si>
+  <si>
+    <t>Número completo do CNPJ do contratante do correspondente - o CNPJ corresponde ao número de inscrição no Cadastro de Pessoa Jurídica. Os oito primeiros números à esquerda (XX. XXX. XXX) formam a "raiz" ou base, que identifica a empresa de forma única. Ex. '50.685.362'. Os 4 próximos números indicam filial. Os últimos dois dígitos são para o número verificador do CNPJ, calculado em duas etapas utilizando o módulo de divisão 11, utilizando-se os 12 primeiros números do CNPJ - inscrição e filial.
+Deve-se ter apenas os números do CNPJ, sem máscara.</t>
   </si>
   <si>
     <t>corporationName</t>
   </si>
   <si>
+    <t>Nome do Correspondente Bancário. Segundo Glossário do
+Bacen: Correspondentes no pais são Empresas, integrantes ou não do Sistema Financeiro Nacional, contratadas por instituições financeiras e demais instituições autorizadas a funcionar pelo Banco Central do Brasil para a prestação de serviços de atendimento aos clientes e usuários dessas instituições. Os correspondentes mais conhecidos são as lotéricas e o banco postal. Ex. 'Empresa Correspondente S.A.'</t>
+  </si>
+  <si>
     <t>groupName</t>
   </si>
   <si>
-    <t>tradingName</t>
-  </si>
-  <si>
-    <t>countrySubDivision</t>
-  </si>
-  <si>
-    <t>Enum</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>areaCode</t>
-  </si>
-  <si>
-    <t>cnpjNumber</t>
-  </si>
-  <si>
-    <t>countryCode</t>
-  </si>
-  <si>
-    <t>allowPublicAccess</t>
+    <t>Nome do conglomerado ao qual pertence o agente bancário, por exemplo: 
+"Companhia Brasileira de Distribuição"
+"Empresa Brasileira de Correios e Telegrafos - ECT"
+'Grupo Pão de Açúcar'</t>
+  </si>
+  <si>
+    <t>Número completo do CNPJ do correspondente - o CNPJ corresponde ao número de inscrição no Cadastro de Pessoa Jurídica. Os oito primeiros números à esquerda (XX. XXX. XXX) formam a "raiz" ou base, que identifica a empresa de forma única. Ex. '50.685.362'. Os 4 próximos números indicam filial. Os últimos dois dígitos são para o número verificador do CNPJ, calculado em duas etapas utilizando o módulo de divisão 11, utilizando-se os 12 primeiros números do CNPJ - inscrição e filial.
+Deve-se ter apenas os números do CNPJ, sem máscara.</t>
+  </si>
+  <si>
+    <t>Logradouro é o termo utilizado pelos Correios para designar uma localidade específica. O logradouro é composto pelo seu tipo seguido dos nomes oficiais. Os tipos de logradouro são: aeroporto, alameda, área, avenida, campo, chácara, colônia, condomínio, conjunto, distrito, esplanada, estação, estrada, fazenda, feira, jardim, ladeira, lago, lagoa ,largo, loteament, núcleo, parque, passarela, pátio, praça, quadra, recanto, residencial, rodovia, rua, setor, sítio, travessa, trecho, trevo, vale, vereda, via, viaduto, viela, vila</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Localidade: O nome da localidade corresponde à designação da cidade ou município no qual o endereço está localizado. Ex. 'São Paulo'
+</t>
+  </si>
+  <si>
+    <t>^(\d{5})-(\d{3})$</t>
   </si>
   <si>
     <r>
@@ -516,6 +481,78 @@
 7 'Recepção e encaminhamento de propostas de fornecimento de cartões de crédito'
 8 'Realização de operações de câmbio'</t>
     </r>
+  </si>
+  <si>
+    <t>1 'Recepção e encaminhamento de propostas de abertura de contas'
+2 'Realização de recebimentos, pagamentos e transferências eletrônicas'
+3 'Recebimentos e pagamentos de qualquer natureza'
+4 'Execução ativa e passiva de ordens de pagamento'
+5 'Recepção e encaminhamento de propostas de operações de crédito e de arrendamento mercantil'
+6 'Recebimento e pagamentos relacionados a letras de câmbio de aceite da instituição'
+7 'Recepção e encaminhamento de propostas de fornecimento de cartões de crédito'
+8 'Realização de operações de câmbio'</t>
+  </si>
+  <si>
+    <t>Nome do conglomerado que disponibiliza os Canais de Atendimento Eletrônico (titular). Ex.  'Organização A'</t>
+  </si>
+  <si>
+    <t>Número completo do CNPJ da instituição responsável pelo canal eletrônico - o CNPJ corresponde ao número de inscrição no Cadastro de Pessoa Jurídica. Os oito primeiros números à esquerda (XX. XXX. XXX) formam a "raiz" ou base, que identifica a empresa de forma única. Ex. '50.685.362'. Os 4 próximos números indicam filial. Os últimos dois dígitos são para o número verificador do CNPJ, calculado em duas etapas utilizando o módulo de divisão 11, utilizando-se os 12 primeiros números do CNPJ - inscrição e filial.
+Deve-se ter apenas os números do CNPJ, sem máscara.</t>
+  </si>
+  <si>
+    <t>Tipo de canal de atendimento:
+1 'Internet banking'
+2 'Mobile banking' 
+3 'Central telefônica banking'
+4 'SAC'
+5 'Ouvidoria'
+6 'Chat'</t>
+  </si>
+  <si>
+    <t>1 'Internet banking'
+2 'Mobile banking' 
+3 'Central telefônica banking'
+4 'SAC'
+5 'Ouvidoria'
+6 'Chat'</t>
+  </si>
+  <si>
+    <t>Números de 0 a 9.
+O Tipo de Canal determina o Tipo de Acesso a ele relacionado: 
+1. URL para acesso ao internet banking,
+2. URL para aquisição do app , 
+3. telefone/URL da central, 
+4. telefone/URL do SAC, 
+5. telefone/URL da ouvidoria, 
+6. telefone/URL para chat</t>
+  </si>
+  <si>
+    <t>countryCode</t>
+  </si>
+  <si>
+    <t>Número de DDI (Discagem Direta Internacional) para  telefone de acesso ao Canal - se houver. Ex. '55'</t>
+  </si>
+  <si>
+    <t>Número de DDD (Discagem Direta à Distância) para  telefone de acesso ao Canal - se houver. Ex. '19'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Número de telefone de acesso ao canal. Ex:' 4004-4828', '99878-5342', '0800-778-7788' 
+</t>
+  </si>
+  <si>
+    <t>^(([0-9]{4,5})-([0-9]{4}))|(([0-9]{4})-([0-9]{3})-([0-9]{4}))$</t>
+  </si>
+  <si>
+    <t>Mensagem complementar necessária para o agrupamento da identificação do telefone. Exemplos relativos ao prenchimento do agrupmento telefone: 
+DDI '55'; DDD '11', '40044828, 'Para clientes no exterior'
+DDI ' ', DDD ' ', 40044828', "Para regiões metropolitanas'
+DDI ' ', DDD ' ', 40044828', "Para demais localidades'</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>Endereço eletrônico de acesso ao canal. URLs são limitadas a 2048 caracteres mas, para o contexto do Sistema Financeiro aberto, será adotado a metade deste tamanho. Ex. 'https://example.com/mobile-banking'</t>
   </si>
   <si>
     <r>
@@ -551,46 +588,12 @@
       <t>.</t>
     </r>
   </si>
-  <si>
-    <t>1-'AC'; 2-'AL'; 3-'AM'; 4-'AP'; 5-'BA'; 6-'CE'; 7-'DF'; 8-'ES'; 9-'GO'; 10-'MA'; 11-'MG'; 12-'MS'; 13-'MT'; 14-'PA'; 15-'PB'; 16-'PE'; 17-'PI'; 18-'PR'; 19-'RJ'; 20-'RN'; 21-'RO'; 22-'RR'; 23-'RS'; 24-'SC'; 25-'SE'; 26-'SP'; 27-'TO'</t>
-  </si>
-  <si>
-    <t>Enumeração referente a cada sigla da unidade da federação que identifica o estado ou o distrito federal, no qual o endereço está localizado. Ex. 1-'AC'. São considerados apenas as siglas para os estados brasileiros.</t>
-  </si>
-  <si>
-    <t>Nome da Instituição, pertencente à organização, responsável pela Dependência. Ex. 'Empresa da Organização A'</t>
-  </si>
-  <si>
-    <t>^(\d{14})$</t>
-  </si>
-  <si>
-    <t>Número completo do CNPJ da instituição responsável pelo canal eletrônico - o CNPJ corresponde ao número de inscrição no Cadastro de Pessoa Jurídica. Os oito primeiros números à esquerda (XX. XXX. XXX) formam a "raiz" ou base, que identifica a empresa de forma única. Ex. '50.685.362'. Os 4 próximos números indicam filial. Os últimos dois dígitos são para o número verificador do CNPJ, calculado em duas etapas utilizando o módulo de divisão 11, utilizando-se os 12 primeiros números do CNPJ - inscrição e filial.
-Deve-se ter apenas os números do CNPJ, sem máscara.</t>
-  </si>
-  <si>
-    <t>Número completo do CNPJ da instituição responsável pela dependência - o CNPJ corresponde ao número de inscrição no Cadastro de Pessoa Jurídica. Os oito primeiros números à esquerda (XX. XXX. XXX) formam a "raiz" ou base, que identifica a empresa de forma única. Ex. '50.685.362'. Os 4 próximos números indicam filial. Os últimos dois dígitos são para o número verificador do CNPJ, calculado em duas etapas utilizando o módulo de divisão 11, utilizando-se os 12 primeiros números do CNPJ - inscrição e filial.
-Deve-se ter apenas os números do CNPJ, sem máscara.</t>
-  </si>
-  <si>
-    <t>Número completo do CNPJ do correspondente - o CNPJ corresponde ao número de inscrição no Cadastro de Pessoa Jurídica. Os oito primeiros números à esquerda (XX. XXX. XXX) formam a "raiz" ou base, que identifica a empresa de forma única. Ex. '50.685.362'. Os 4 próximos números indicam filial. Os últimos dois dígitos são para o número verificador do CNPJ, calculado em duas etapas utilizando o módulo de divisão 11, utilizando-se os 12 primeiros números do CNPJ - inscrição e filial.
-Deve-se ter apenas os números do CNPJ, sem máscara.</t>
-  </si>
-  <si>
-    <t>Número completo do CNPJ do contratante do correspondente - o CNPJ corresponde ao número de inscrição no Cadastro de Pessoa Jurídica. Os oito primeiros números à esquerda (XX. XXX. XXX) formam a "raiz" ou base, que identifica a empresa de forma única. Ex. '50.685.362'. Os 4 próximos números indicam filial. Os últimos dois dígitos são para o número verificador do CNPJ, calculado em duas etapas utilizando o módulo de divisão 11, utilizando-se os 12 primeiros números do CNPJ - inscrição e filial.
-Deve-se ter apenas os números do CNPJ, sem máscara.</t>
-  </si>
-  <si>
-    <t>^(\d{1})$</t>
-  </si>
-  <si>
-    <t>Números de 0 a 9.</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1051,17 +1054,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="97.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" style="7" customWidth="1"/>
@@ -1077,7 +1080,7 @@
     <col min="12" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1113,25 +1116,25 @@
       </c>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="17.25" customHeight="1">
       <c r="A2" s="3" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/",B2)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/name</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="13">
         <v>30</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>15</v>
@@ -1144,29 +1147,29 @@
         <v>1</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L2" s="11"/>
     </row>
-    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="30">
       <c r="A3" s="3" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/",B3)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/name</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>112</v>
+        <v>17</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="13">
         <v>30</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>15</v>
@@ -1179,35 +1182,35 @@
         <v>1</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L3" s="11"/>
     </row>
-    <row r="4" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="105">
       <c r="A4" s="3" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/",B4)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/cnpjNumber</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>115</v>
+        <v>19</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="13">
         <v>14</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>113</v>
+        <v>20</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>119</v>
+        <v>21</v>
       </c>
       <c r="I4" s="9">
         <v>1</v>
@@ -1216,35 +1219,35 @@
         <v>1</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L4" s="11"/>
     </row>
-    <row r="5" spans="1:12" ht="285" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="285">
       <c r="A5" s="3" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/branches/identification/",B5)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/identification/type</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="E5" s="13">
         <v>2</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="I5" s="13">
         <v>1</v>
@@ -1253,35 +1256,35 @@
         <v>3</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L5" s="11"/>
     </row>
-    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="45">
       <c r="A6" s="3" t="str">
         <f t="shared" ref="A6:A8" si="0">CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/branches/identification/",B6)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/identification/code</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="13">
         <v>4</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I6" s="9">
         <v>1</v>
@@ -1290,60 +1293,60 @@
         <v>1</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="L6" s="11"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/identification/checkDigit</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" s="13">
         <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L7" s="11"/>
     </row>
-    <row r="8" spans="1:12" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="90.75" customHeight="1">
       <c r="A8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/identification/name</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="13">
         <v>100</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>15</v>
@@ -1356,35 +1359,35 @@
         <v>1</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L8" s="11"/>
     </row>
-    <row r="9" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="105">
       <c r="A9" s="3" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/branches/postalAddress/",B9)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/postalAddress/streetType</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>85</v>
+        <v>37</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="15">
         <v>10</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I9" s="9">
         <v>1</v>
@@ -1393,29 +1396,29 @@
         <v>1</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L9" s="11"/>
     </row>
-    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="45">
       <c r="A10" s="3" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/branches/postalAddress/",B10)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/postalAddress/streetName</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="15">
         <v>50</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>15</v>
@@ -1428,29 +1431,29 @@
         <v>1</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L10" s="11"/>
     </row>
-    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="30">
       <c r="A11" s="3" t="str">
         <f t="shared" ref="A11:A16" si="1">CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/branches/postalAddress/",B11)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/postalAddress/buildingNumber</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" s="15">
         <v>6</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>15</v>
@@ -1463,29 +1466,29 @@
         <v>1</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L11" s="11"/>
     </row>
-    <row r="12" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="33.75" customHeight="1">
       <c r="A12" s="3" t="str">
         <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/postalAddress/additionalInfo</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" s="15">
         <v>30</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>15</v>
@@ -1498,29 +1501,29 @@
         <v>1</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L12" s="11"/>
     </row>
-    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="30">
       <c r="A13" s="3" t="str">
         <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/postalAddress/districtName</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E13" s="13">
         <v>50</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>15</v>
@@ -1533,29 +1536,29 @@
         <v>1</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L13" s="11"/>
     </row>
-    <row r="14" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="34.5" customHeight="1">
       <c r="A14" s="3" t="str">
         <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/postalAddress/townName</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E14" s="15">
         <v>50</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>15</v>
@@ -1568,35 +1571,35 @@
         <v>1</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L14" s="11"/>
     </row>
-    <row r="15" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="60">
       <c r="A15" s="3" t="str">
         <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/postalAddress/countrySubDivision</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>101</v>
+        <v>50</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>111</v>
+        <v>51</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="E15" s="13">
         <v>2</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>118</v>
+        <v>52</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>110</v>
+        <v>53</v>
       </c>
       <c r="I15" s="9">
         <v>1</v>
@@ -1605,32 +1608,32 @@
         <v>1</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L15" s="11"/>
     </row>
-    <row r="16" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="75">
       <c r="A16" s="3" t="str">
         <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/postalAddress/postCode</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="E16" s="13">
         <v>9</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="9">
@@ -1640,35 +1643,35 @@
         <v>1</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L16" s="11"/>
     </row>
-    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="30">
       <c r="A17" s="3" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/branches/availability/standard/",B17)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/availability/standard/weekday</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E17" s="13">
         <v>13</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="I17" s="9">
         <v>1</v>
@@ -1677,32 +1680,32 @@
         <v>1</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L17" s="11"/>
     </row>
-    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="30">
       <c r="A18" s="3" t="str">
         <f t="shared" ref="A18:A24" si="2">CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/branches/availability/standard/",B18)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/availability/standard/openingTime</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E18" s="13">
         <v>13</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="9">
@@ -1712,32 +1715,32 @@
         <v>1</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="L18" s="11"/>
     </row>
-    <row r="19" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="33" customHeight="1">
       <c r="A19" s="3" t="str">
         <f t="shared" si="2"/>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/availability/standard/closingTime</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E19" s="13">
         <v>13</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="9">
@@ -1747,29 +1750,29 @@
         <v>1</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="L19" s="11"/>
     </row>
-    <row r="20" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="32.25" customHeight="1">
       <c r="A20" s="3" t="str">
         <f t="shared" si="2"/>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/availability/standard/exceptionAvailability</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E20" s="13">
         <v>2000</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>15</v>
@@ -1782,35 +1785,35 @@
         <v>1</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L20" s="11"/>
     </row>
-    <row r="21" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="45">
       <c r="A21" s="3" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/branches/availability/standard/",B21)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/availability/standard/allowPublicAccess</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E21" s="13">
         <v>1</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I21" s="9">
         <v>1</v>
@@ -1819,142 +1822,142 @@
         <v>1</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L21" s="11"/>
     </row>
-    <row r="22" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="45">
       <c r="A22" s="3" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/branches/availability/phones/",B22)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/availability/phones/type</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="E22" s="13">
         <v>1</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="I22" s="9">
         <v>0</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="L22" s="11"/>
     </row>
-    <row r="23" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="30">
       <c r="A23" s="3" t="str">
         <f t="shared" ref="A23:A24" si="3">CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/branches/availability/phones/",B23)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/availability/phones/areaCode</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>20</v>
+        <v>81</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E23" s="13">
         <v>2</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="9">
         <v>0</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="L23" s="11"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" s="3" t="str">
         <f t="shared" si="3"/>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/availability/phones/number</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E24" s="13">
         <v>10</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="9">
         <v>0</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L24" s="11"/>
     </row>
-    <row r="25" spans="1:12" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="142.5" customHeight="1">
       <c r="A25" s="3" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/branches/service/",B25)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/service/codes</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="E25" s="13">
         <v>2</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="I25" s="9">
         <v>1</v>
@@ -1963,29 +1966,29 @@
         <v>8</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L25" s="11"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" s="3" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/branches/service/",B26)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/branches/service/additionalInfo</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>13</v>
+        <v>90</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E26" s="13">
         <v>2000</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>15</v>
@@ -1998,11 +2001,11 @@
         <v>1</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L26" s="11"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="8"/>
@@ -2023,17 +2026,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="I7" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="101.5703125" style="27" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" style="34" customWidth="1"/>
@@ -2049,7 +2052,7 @@
     <col min="12" max="16384" width="9.140625" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -2084,25 +2087,25 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="47.25" customHeight="1">
       <c r="A2" s="1" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/",B2)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/name</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="24">
         <v>30</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G2" s="23" t="s">
         <v>15</v>
@@ -2115,28 +2118,28 @@
         <v>1</v>
       </c>
       <c r="K2" s="26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="7" customFormat="1" ht="30">
       <c r="A3" s="3" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/",B3)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/name</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>112</v>
+        <v>17</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="13">
         <v>30</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>15</v>
@@ -2149,35 +2152,35 @@
         <v>1</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L3" s="11"/>
     </row>
-    <row r="4" spans="1:12" s="7" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="7" customFormat="1" ht="150">
       <c r="A4" s="3" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/",B4)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/cnpjNumber</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>115</v>
+        <v>19</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="13">
         <v>14</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>113</v>
+        <v>20</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>119</v>
+        <v>21</v>
       </c>
       <c r="I4" s="9">
         <v>1</v>
@@ -2186,29 +2189,29 @@
         <v>1</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L4" s="11"/>
     </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="30">
       <c r="A5" s="1" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/contractors/",B5)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/name</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="24">
         <v>30</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G5" s="23" t="s">
         <v>15</v>
@@ -2221,34 +2224,34 @@
         <v>1</v>
       </c>
       <c r="K5" s="26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="64.5" customHeight="1">
       <c r="A6" s="1" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/contractors/",B6)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/cnpjNumber</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="13">
         <v>14</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>113</v>
+        <v>20</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>119</v>
+        <v>21</v>
       </c>
       <c r="I6" s="9">
         <v>1</v>
@@ -2257,28 +2260,28 @@
         <v>1</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="118.5" customHeight="1">
       <c r="A7" s="1" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/identification/",B7)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/identification/corporationName</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" s="24">
         <v>100</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G7" s="23" t="s">
         <v>15</v>
@@ -2288,136 +2291,136 @@
         <v>1</v>
       </c>
       <c r="J7" s="24" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="K7" s="28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="71.25" customHeight="1">
       <c r="A8" s="1" t="str">
-        <f t="shared" ref="A8:A10" si="0">CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/identification/",B8)</f>
+        <f t="shared" ref="A8:A9" si="0">CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/identification/",B8)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/identification/groupName</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="24">
         <v>100</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="G8" s="23" t="s">
         <v>15</v>
       </c>
       <c r="H8" s="25"/>
       <c r="I8" s="24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="24">
         <v>1</v>
       </c>
       <c r="K8" s="26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="78.75" customHeight="1">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/identification/tradingName</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="24">
-        <v>100</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="23" t="s">
+        <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/identification/cnpjNumber</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="13">
+        <v>14</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="9">
+        <v>1</v>
+      </c>
+      <c r="J9" s="9">
+        <v>1</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" ht="135.75" customHeight="1">
+      <c r="A10" s="1" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/postalAdress/",B10)</f>
+        <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/postalAdress/streetType</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="24">
+        <v>10</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="25"/>
-      <c r="I9" s="24">
-        <v>1</v>
-      </c>
-      <c r="J9" s="24">
-        <v>1</v>
-      </c>
-      <c r="K9" s="29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/identification/cnpjNumber</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="13">
-        <v>14</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="I10" s="9">
-        <v>1</v>
-      </c>
-      <c r="J10" s="9">
-        <v>1</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="L10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="25"/>
+      <c r="I10" s="30">
+        <v>1</v>
+      </c>
+      <c r="J10" s="30">
+        <v>1</v>
+      </c>
+      <c r="K10" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="60">
       <c r="A11" s="1" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/postalAdress/",B11)</f>
-        <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/postalAdress/streetType</v>
+        <f t="shared" ref="A11:A17" si="1">CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/postalAdress/",B11)</f>
+        <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/postalAdress/streetName</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" s="24">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G11" s="23" t="s">
         <v>15</v>
@@ -2430,62 +2433,62 @@
         <v>1</v>
       </c>
       <c r="K11" s="29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="45">
       <c r="A12" s="1" t="str">
-        <f t="shared" ref="A12:A18" si="1">CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/postalAdress/",B12)</f>
-        <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/postalAdress/streetName</v>
+        <f t="shared" si="1"/>
+        <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/postalAdress/buildingNumber</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" s="24">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G12" s="23" t="s">
         <v>15</v>
       </c>
       <c r="H12" s="25"/>
-      <c r="I12" s="30">
-        <v>1</v>
-      </c>
-      <c r="J12" s="30">
+      <c r="I12" s="24">
+        <v>1</v>
+      </c>
+      <c r="J12" s="24">
         <v>1</v>
       </c>
       <c r="K12" s="29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="45">
       <c r="A13" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/postalAdress/buildingNumber</v>
+        <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/postalAdress/additionalInfo</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>87</v>
+        <v>44</v>
       </c>
       <c r="C13" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="24">
         <v>30</v>
       </c>
-      <c r="D13" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="24">
-        <v>6</v>
-      </c>
       <c r="F13" s="23" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="G13" s="23" t="s">
         <v>15</v>
@@ -2498,28 +2501,28 @@
         <v>1</v>
       </c>
       <c r="K13" s="29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="45">
       <c r="A14" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/postalAdress/additionalInfo</v>
+        <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/postalAdress/districtName</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>88</v>
+        <v>46</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E14" s="24">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G14" s="23" t="s">
         <v>15</v>
@@ -2532,28 +2535,28 @@
         <v>1</v>
       </c>
       <c r="K14" s="29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="45.75" customHeight="1">
       <c r="A15" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/postalAdress/districtName</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/postalAdress/",B15)</f>
+        <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/postalAdress/townName</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15" s="24">
         <v>50</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G15" s="23" t="s">
         <v>15</v>
@@ -2566,33 +2569,33 @@
         <v>1</v>
       </c>
       <c r="K15" s="29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="60">
       <c r="A16" s="1" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/postalAdress/",B16)</f>
-        <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/postalAdress/townName</v>
+        <f t="shared" si="1"/>
+        <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/postalAdress/countrySubDivision</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>14</v>
+        <v>50</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>24</v>
       </c>
       <c r="E16" s="24">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="25"/>
+        <v>14</v>
+      </c>
+      <c r="G16" s="23"/>
+      <c r="H16" s="26" t="s">
+        <v>53</v>
+      </c>
       <c r="I16" s="24">
         <v>1</v>
       </c>
@@ -2600,148 +2603,127 @@
         <v>1</v>
       </c>
       <c r="K16" s="29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="94.5" customHeight="1">
       <c r="A17" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/postalAdress/countrySubDivision</v>
+        <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/postalAdress/postCode</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="24">
+        <v>9</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="D17" s="31" t="s">
+      <c r="H17" s="25"/>
+      <c r="I17" s="30">
+        <v>1</v>
+      </c>
+      <c r="J17" s="30">
+        <v>1</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="225">
+      <c r="A18" s="1" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/service/",B18)</f>
+        <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/service/codes</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="E17" s="24">
+      <c r="D18" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="24">
         <v>2</v>
       </c>
-      <c r="F17" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="23"/>
-      <c r="H17" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="I17" s="24">
-        <v>1</v>
-      </c>
-      <c r="J17" s="24">
-        <v>1</v>
-      </c>
-      <c r="K17" s="29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/postalAdress/postCode</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C18" s="29" t="s">
+      <c r="F18" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="24">
-        <v>9</v>
-      </c>
-      <c r="F18" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="H18" s="25"/>
+      <c r="H18" s="26" t="s">
+        <v>103</v>
+      </c>
       <c r="I18" s="30">
         <v>1</v>
       </c>
       <c r="J18" s="30">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K18" s="29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="225" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="1" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/service/",B19)</f>
-        <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/service/codes</v>
+        <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/service/additionalInfo</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C19" s="29" t="s">
-        <v>108</v>
+        <v>44</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>102</v>
+        <v>13</v>
       </c>
       <c r="E19" s="24">
-        <v>2</v>
+        <v>2000</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="H19" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="I19" s="30">
-        <v>1</v>
-      </c>
-      <c r="J19" s="30">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="H19" s="25"/>
+      <c r="I19" s="24">
+        <v>0</v>
+      </c>
+      <c r="J19" s="24">
+        <v>1</v>
       </c>
       <c r="K19" s="29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/service/",B20)</f>
-        <v>openBankingBrazil/&lt;Organisation&gt;/companies/contractors/bankingAgents/service/additionalInfo</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="24">
-        <v>2000</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" s="25"/>
-      <c r="I20" s="24">
-        <v>0</v>
-      </c>
-      <c r="J20" s="24">
-        <v>1</v>
-      </c>
-      <c r="K20" s="29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="29"/>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2754,12 +2736,12 @@
       <c r="J21" s="33"/>
       <c r="K21" s="29"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="32"/>
+      <c r="E22" s="33"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -2767,7 +2749,7 @@
       <c r="J22" s="33"/>
       <c r="K22" s="29"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2780,7 +2762,7 @@
       <c r="J23" s="33"/>
       <c r="K23" s="29"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2793,7 +2775,7 @@
       <c r="J24" s="33"/>
       <c r="K24" s="29"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2806,7 +2788,7 @@
       <c r="J25" s="33"/>
       <c r="K25" s="29"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2819,7 +2801,7 @@
       <c r="J26" s="33"/>
       <c r="K26" s="29"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2832,7 +2814,7 @@
       <c r="J27" s="33"/>
       <c r="K27" s="29"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2845,7 +2827,7 @@
       <c r="J28" s="33"/>
       <c r="K28" s="29"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2858,7 +2840,7 @@
       <c r="J29" s="33"/>
       <c r="K29" s="29"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2871,7 +2853,7 @@
       <c r="J30" s="33"/>
       <c r="K30" s="29"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2884,7 +2866,7 @@
       <c r="J31" s="33"/>
       <c r="K31" s="29"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2897,7 +2879,7 @@
       <c r="J32" s="33"/>
       <c r="K32" s="29"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2910,7 +2892,7 @@
       <c r="J33" s="33"/>
       <c r="K33" s="29"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2923,7 +2905,7 @@
       <c r="J34" s="33"/>
       <c r="K34" s="29"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2936,7 +2918,7 @@
       <c r="J35" s="33"/>
       <c r="K35" s="29"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2949,7 +2931,7 @@
       <c r="J36" s="33"/>
       <c r="K36" s="29"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2962,7 +2944,7 @@
       <c r="J37" s="33"/>
       <c r="K37" s="29"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2975,7 +2957,7 @@
       <c r="J38" s="33"/>
       <c r="K38" s="29"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2988,7 +2970,7 @@
       <c r="J39" s="33"/>
       <c r="K39" s="29"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3001,7 +2983,7 @@
       <c r="J40" s="33"/>
       <c r="K40" s="29"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3014,7 +2996,7 @@
       <c r="J41" s="33"/>
       <c r="K41" s="29"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -3027,7 +3009,7 @@
       <c r="J42" s="33"/>
       <c r="K42" s="29"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -3040,7 +3022,7 @@
       <c r="J43" s="33"/>
       <c r="K43" s="29"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -3053,19 +3035,6 @@
       <c r="J44" s="33"/>
       <c r="K44" s="29"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="33"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="33"/>
-      <c r="K45" s="29"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3073,17 +3042,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="97.5703125" style="27" customWidth="1"/>
     <col min="2" max="2" width="22.140625" style="39" customWidth="1"/>
@@ -3099,7 +3068,7 @@
     <col min="12" max="16384" width="9.140625" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="37" customFormat="1">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -3134,25 +3103,25 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="30">
       <c r="A2" s="1" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/",B2)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/name</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>71</v>
+        <v>104</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="24">
         <v>30</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>15</v>
@@ -3165,28 +3134,28 @@
         <v>1</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="7" customFormat="1" ht="45">
       <c r="A3" s="3" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/",B3)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/name</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>112</v>
+        <v>17</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="13">
         <v>30</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>15</v>
@@ -3199,35 +3168,35 @@
         <v>1</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L3" s="11"/>
     </row>
-    <row r="4" spans="1:12" s="7" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="7" customFormat="1" ht="165">
       <c r="A4" s="3" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/",B4)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/cnpjNumber</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>114</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="13">
         <v>14</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>113</v>
+        <v>20</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>119</v>
+        <v>21</v>
       </c>
       <c r="I4" s="9">
         <v>1</v>
@@ -3236,35 +3205,35 @@
         <v>1</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L4" s="11"/>
     </row>
-    <row r="5" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="150">
       <c r="A5" s="1" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/channels/Identification/",B5)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/channels/Identification/type</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>59</v>
+        <v>106</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="E5" s="24">
         <v>2</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>60</v>
+        <v>107</v>
       </c>
       <c r="I5" s="24">
         <v>1</v>
@@ -3273,131 +3242,131 @@
         <v>6</v>
       </c>
       <c r="K5" s="18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30">
       <c r="A6" s="1" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/channels/identification/phones/",B6)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/channels/identification/phones/countryCode</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>54</v>
+        <v>110</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="24">
         <v>2</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="H6" s="38"/>
       <c r="I6" s="24">
         <v>0</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="K6" s="26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="30">
       <c r="A7" s="1" t="str">
         <f t="shared" ref="A7:A9" si="0">CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/channels/identification/phones/",B7)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/channels/identification/phones/areaCode</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" s="24">
         <v>2</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="24">
         <v>0</v>
       </c>
       <c r="J7" s="24" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="K7" s="26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="29.25" customHeight="1">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/channels/identification/phones/number</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="24">
         <v>13</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="24">
         <v>0</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="K8" s="26" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="90" customHeight="1">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/channels/identification/phones/additionalInfo</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>64</v>
+        <v>114</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="24">
         <v>50</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="G9" s="23" t="s">
         <v>15</v>
@@ -3407,32 +3376,32 @@
         <v>0</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="K9" s="26" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="60">
       <c r="A10" s="1" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/channels/identification/",B10)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/channels/identification/url</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>55</v>
+        <v>116</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="24">
         <v>1024</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="G10" s="23" t="s">
         <v>15</v>
@@ -3442,38 +3411,38 @@
         <v>0</v>
       </c>
       <c r="J10" s="24" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="K10" s="26" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" ht="179.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="179.25" customHeight="1">
       <c r="A11" s="1" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/channels/service/",B11)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/channels/service/codes</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="E11" s="24">
         <v>2</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="I11" s="24">
         <v>1</v>
@@ -3482,28 +3451,28 @@
         <v>7</v>
       </c>
       <c r="K11" s="26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="1" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;Organisation&gt;/companies/channels/service/",B12)</f>
         <v>openBankingBrazil/&lt;Organisation&gt;/companies/channels/service/additionalInfo</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>13</v>
+        <v>90</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" s="24">
         <v>2000</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>15</v>
@@ -3516,10 +3485,10 @@
         <v>1</v>
       </c>
       <c r="K12" s="29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="1"/>
       <c r="B13" s="38"/>
       <c r="C13" s="1"/>
@@ -3532,7 +3501,7 @@
       <c r="J13" s="33"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" s="1"/>
       <c r="B14" s="38"/>
       <c r="C14" s="1"/>

</xml_diff>

<commit_message>
alteracoes no dicionario de dados e no slate
</commit_message>
<xml_diff>
--- a/DicionarioDeDados-DependenciasCorrespondentesCanais.xlsx
+++ b/DicionarioDeDados-DependenciasCorrespondentesCanais.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erdxbpo\OneDrive - Banco Itaú SA\Documentos\AD\OpenBankingData\Febraban\DataOwner\DicionáriosOficiais\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loro\source\openbanking-febraban\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{A0D46A99-A67C-4FA2-BDDB-27039DBF723D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{C843219E-291A-4910-A17D-8EC5E37CF55F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540B1E0B-6FCF-4CD6-8C3E-A23D791641A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="6885" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dependências-Agências" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="CanaisAtendimentoEletrônico " sheetId="4" r:id="rId3"/>
     <sheet name="Canaistelefônicos" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1182,10 +1184,10 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1880,8 +1882,8 @@
     </row>
     <row r="20" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/branches/availability/standard/",B20)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/branches/availability/standard/exceptionAvailability</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/branches/availability/",B20)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/branches/availability/exceptionAvailability</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>55</v>
@@ -1915,8 +1917,8 @@
     </row>
     <row r="21" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/branches/availability/standard/",B21)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/branches/availability/standard/allowPublicAccess</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/branches/availability/",B21)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/branches/availability/allowPublicAccess</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>57</v>

</xml_diff>